<commit_message>
completed computation scratch & started c program
</commit_message>
<xml_diff>
--- a/daily learning.xlsx
+++ b/daily learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\self learning\daily-learning-skills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8701EA-7236-46F9-9EB1-524E60E3D76F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19723073-3C1B-480D-9D11-A8199B887B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Daily learning</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>computational thinking,scratch</t>
+  </si>
+  <si>
+    <t>complete on date</t>
+  </si>
+  <si>
+    <t>complete on time</t>
+  </si>
+  <si>
+    <t>writing program in c</t>
   </si>
 </sst>
 </file>
@@ -374,19 +383,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -402,8 +412,14 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -412,12 +428,37 @@
       </c>
       <c r="C2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43774</v>
+        <v>43775</v>
       </c>
       <c r="D2" s="2">
         <v>0.92499999999999993</v>
       </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43775</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43775</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.46597222222222223</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>